<commit_message>
Unificação do teste de cadastro
</commit_message>
<xml_diff>
--- a/target/classes/br/com/rsinet/HUB_TDD/DadosTeste/DadosTeste.xlsx
+++ b/target/classes/br/com/rsinet/HUB_TDD/DadosTeste/DadosTeste.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4DFE0655-9ACF-4AA3-B204-9191C63BB9F3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{79DDA293-C99B-4F27-9B73-440B3D1F4CB7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="20790" windowHeight="11820" xr2:uid="{C5C229D6-6427-449A-9BBF-D07F863B75D3}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="20790" windowHeight="11820" xr2:uid="{C5C229D6-6427-449A-9BBF-D07F863B75D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -129,7 +129,7 @@
     <t>usertests356</t>
   </si>
   <si>
-    <t>usertests3880</t>
+    <t>usertests3882</t>
   </si>
 </sst>
 </file>
@@ -543,7 +543,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Unificação de alguns testes e pequenas refatorações
</commit_message>
<xml_diff>
--- a/target/classes/br/com/rsinet/HUB_TDD/DadosTeste/DadosTeste.xlsx
+++ b/target/classes/br/com/rsinet/HUB_TDD/DadosTeste/DadosTeste.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{79DDA293-C99B-4F27-9B73-440B3D1F4CB7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2C5AF299-470F-4629-8F33-5B3C47489342}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="20790" windowHeight="11820" xr2:uid="{C5C229D6-6427-449A-9BBF-D07F863B75D3}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="20880" windowHeight="22215" xr2:uid="{C5C229D6-6427-449A-9BBF-D07F863B75D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J7"/>
+  <oleSize ref="A1:J14"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>Nome Caso de Teste</t>
   </si>
@@ -129,7 +129,7 @@
     <t>usertests356</t>
   </si>
   <si>
-    <t>usertests3882</t>
+    <t>usertests3884</t>
   </si>
 </sst>
 </file>
@@ -543,13 +543,13 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="6" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -687,10 +687,25 @@
         <v>33</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="C6" s="5"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
       <c r="J9" s="5"/>
     </row>
   </sheetData>
@@ -708,7 +723,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>